<commit_message>
Ajuste das siglas que identificam as fontes de dados.
</commit_message>
<xml_diff>
--- a/DataBase/VHF_NAV_.xlsx
+++ b/DataBase/VHF_NAV_.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Downloads\PMEC 2022\PmecDB\DataBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric\Documents\PmecDB\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76E187FD-8AD9-4AE4-9A88-62FCF21CB87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{770E9A1E-B7B1-41B6-86F5-A716463C4C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20580" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>